<commit_message>
finish processing the four Burnham spreadsheets
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/BurnhamAssays/Burnham Center for Chemical Genomics_edited_20120910_TC_red.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/BurnhamAssays/Burnham Center for Chemical Genomics_edited_20120910_TC_red.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="399">
   <si>
     <t>Instructions:
 Fill out from left to right.  Watch for red errors, correct them before moving on to the next column</t>
@@ -980,9 +980,6 @@
   </si>
   <si>
     <t>OMFP</t>
-  </si>
-  <si>
-    <t>fold dilution</t>
   </si>
   <si>
     <t>GI:12044</t>
@@ -2624,8 +2621,8 @@
   <dimension ref="A1:BB99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U25" sqref="U25"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3728,13 +3725,13 @@
         <v>201</v>
       </c>
       <c r="D11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E11" t="s">
         <v>219</v>
       </c>
       <c r="F11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G11" t="s">
         <v>262</v>
@@ -3743,7 +3740,7 @@
         <v>258</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J11" s="10">
         <v>5000</v>
@@ -3752,13 +3749,13 @@
         <v>249</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AC11" s="5" t="s">
         <v>282</v>
@@ -3837,20 +3834,16 @@
       <c r="H12" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J12">
-        <v>200</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="J12"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
@@ -3866,19 +3859,19 @@
         <v>255</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J13" s="8">
         <v>1</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>210</v>
@@ -3932,20 +3925,15 @@
       <c r="H14" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J14" s="8">
-        <v>200</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="K14" s="9"/>
       <c r="L14" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>210</v>
@@ -4000,7 +3988,7 @@
         <v>270</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J15" s="20">
         <v>150</v>
@@ -4009,7 +3997,7 @@
         <v>246</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M15" s="21" t="s">
         <v>238</v>
@@ -4029,13 +4017,13 @@
         <v>201</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>219</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>262</v>
@@ -4044,7 +4032,7 @@
         <v>258</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J16" s="10">
         <v>5000</v>
@@ -4053,13 +4041,13 @@
         <v>249</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -4164,20 +4152,15 @@
       <c r="H17" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J17" s="8">
-        <v>200</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="K17" s="9"/>
       <c r="L17" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
@@ -4193,19 +4176,19 @@
         <v>255</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J18" s="8">
         <v>1</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>210</v>
@@ -4259,20 +4242,15 @@
       <c r="H19" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J19" s="8">
-        <v>200</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="K19" s="9"/>
       <c r="L19" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>210</v>
@@ -4327,7 +4305,7 @@
         <v>270</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J20" s="20">
         <v>150</v>
@@ -4336,7 +4314,7 @@
         <v>246</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M20" s="21" t="s">
         <v>238</v>
@@ -4356,13 +4334,13 @@
         <v>201</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E21" s="38" t="s">
         <v>219</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>262</v>
@@ -4371,7 +4349,7 @@
         <v>258</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J21" s="10">
         <v>5000</v>
@@ -4380,13 +4358,13 @@
         <v>249</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
@@ -4491,20 +4469,15 @@
       <c r="H22" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J22" s="8">
-        <v>200</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="K22" s="9"/>
       <c r="L22" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
@@ -4520,19 +4493,19 @@
         <v>255</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J23" s="8">
         <v>1</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O23" s="8" t="s">
         <v>210</v>
@@ -4541,7 +4514,7 @@
         <v>213</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R23" s="8" t="s">
         <v>206</v>
@@ -4586,20 +4559,15 @@
       <c r="H24" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="J24" s="20">
-        <v>200</v>
-      </c>
-      <c r="K24" s="21" t="s">
-        <v>314</v>
-      </c>
+      <c r="K24" s="21"/>
       <c r="L24" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O24" s="20" t="s">
         <v>210</v>
@@ -4608,7 +4576,7 @@
         <v>213</v>
       </c>
       <c r="Q24" s="20" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R24" s="20" t="s">
         <v>206</v>
@@ -4652,7 +4620,7 @@
         <v>#REF!</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>216</v>
@@ -4664,7 +4632,7 @@
         <v>271</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J25" s="20">
         <v>32</v>
@@ -4673,13 +4641,13 @@
         <v>212</v>
       </c>
       <c r="L25" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M25" s="20" t="s">
         <v>238</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O25" s="20" t="s">
         <v>210</v>
@@ -4688,7 +4656,7 @@
         <v>254</v>
       </c>
       <c r="Q25" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R25" s="20" t="s">
         <v>206</v>
@@ -4700,7 +4668,7 @@
         <v>200</v>
       </c>
       <c r="U25" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Y25" s="21" t="s">
         <v>275</v>
@@ -4784,13 +4752,13 @@
       </c>
       <c r="B26" t="str">
         <f t="shared" ref="B26:B59" si="0">IF(OR($A25=$A26,ISBLANK($A26)),"",IF(ISERR(SEARCH("cell-based",E26)),IF(AND(ISERR(SEARCH("biochem",E26)),ISERR(SEARCH("protein",E26)),ISERR(SEARCH("nucleic",E26))),"",IF(ISERR(SEARCH("target",G26)),"Define a Target component","")),IF(ISERR(SEARCH("cell",G26)),"Define a Cell component",""))&amp;IF(ISERR(SEARCH("small-molecule",E26)),IF(ISBLANK(K26), "Need a Detector Role",""),"")&amp;IF(ISERR(SEARCH("fluorescence",L26)),"",IF(ISBLANK(S26), "Need Emission",IF(ISBLANK(R26), "Need Excitation","")))&amp;IF(ISERR(SEARCH("absorbance",L26)),"",IF(ISBLANK(T26), "Need Absorbance","")))</f>
-        <v/>
+        <v>Need a Detector Role</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>230</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>215</v>
@@ -4805,22 +4773,18 @@
         <v>270</v>
       </c>
       <c r="I26" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="J26" s="8">
-        <v>1000</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
@@ -4926,7 +4890,7 @@
         <v>273</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J27" s="8">
         <v>0.5</v>
@@ -4935,7 +4899,7 @@
         <v>225</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>226</v>
@@ -4952,7 +4916,7 @@
         <v>273</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J28" s="8">
         <v>1</v>
@@ -4961,7 +4925,7 @@
         <v>225</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:54" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4976,7 +4940,7 @@
         <v>273</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J29" s="8">
         <v>1000</v>
@@ -4985,7 +4949,7 @@
         <v>225</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:54" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -5000,10 +4964,10 @@
         <v>273</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>210</v>
@@ -5051,7 +5015,7 @@
         <v>230</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>215</v>
@@ -5066,22 +5030,18 @@
         <v>270</v>
       </c>
       <c r="I31" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="J31" s="8">
-        <v>1000</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
@@ -5188,7 +5148,7 @@
         <v>273</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J32" s="8">
         <v>0.5</v>
@@ -5197,7 +5157,7 @@
         <v>225</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O32" s="8" t="s">
         <v>210</v>
@@ -5248,7 +5208,7 @@
         <v>273</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J33" s="8">
         <v>1</v>
@@ -5257,7 +5217,7 @@
         <v>225</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="34" spans="1:54" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -5272,7 +5232,7 @@
         <v>273</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J34" s="20">
         <v>1000</v>
@@ -5281,7 +5241,7 @@
         <v>225</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.2">
@@ -5296,7 +5256,7 @@
         <v>218</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>215</v>
@@ -5311,7 +5271,7 @@
         <v>270</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J35" s="10">
         <v>3.7</v>
@@ -5320,13 +5280,13 @@
         <v>229</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -5447,13 +5407,13 @@
         <v>229</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O36" s="8" t="s">
         <v>210</v>
@@ -5583,10 +5543,10 @@
         <v>229</v>
       </c>
       <c r="L37" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O37" s="20" t="s">
         <v>210</v>
@@ -5618,7 +5578,7 @@
         <v>201</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>219</v>
@@ -5631,7 +5591,7 @@
         <v>265</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J38" s="8">
         <v>7500</v>
@@ -5640,13 +5600,13 @@
         <v>249</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
@@ -5747,14 +5707,9 @@
       <c r="H39" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="J39" s="8">
-        <v>8</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>314</v>
-      </c>
+      <c r="K39" s="9"/>
       <c r="N39" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>226</v>
@@ -5802,14 +5757,9 @@
       <c r="H40" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="J40" s="20">
-        <v>10</v>
-      </c>
-      <c r="K40" s="21" t="s">
-        <v>314</v>
-      </c>
+      <c r="K40" s="21"/>
       <c r="N40" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AC40" s="24"/>
       <c r="AD40" s="18"/>
@@ -5820,7 +5770,7 @@
       </c>
       <c r="B41" t="str">
         <f>IF(OR($A38=$A41,ISBLANK($A41)),"",IF(ISERR(SEARCH("cell-based",E41)),IF(AND(ISERR(SEARCH("biochem",E41)),ISERR(SEARCH("protein",E41)),ISERR(SEARCH("nucleic",E41))),"",IF(ISERR(SEARCH("target",G41)),"Define a Target component","")),IF(ISERR(SEARCH("cell",G41)),"Define a Cell component",""))&amp;IF(ISERR(SEARCH("small-molecule",E41)),IF(ISBLANK(K41), "Need a Detector Role",""),"")&amp;IF(ISERR(SEARCH("fluorescence",L41)),"",IF(ISBLANK(S41), "Need Emission",IF(ISBLANK(R41), "Need Excitation","")))&amp;IF(ISERR(SEARCH("absorbance",L41)),"",IF(ISBLANK(T41), "Need Absorbance","")))</f>
-        <v/>
+        <v>Need a Detector Role</v>
       </c>
       <c r="C41" t="s">
         <v>230</v>
@@ -5837,17 +5787,13 @@
       <c r="H41" t="s">
         <v>222</v>
       </c>
-      <c r="J41" s="25">
-        <v>3.5</v>
-      </c>
-      <c r="K41" s="27" t="s">
-        <v>314</v>
-      </c>
+      <c r="J41" s="25"/>
+      <c r="K41" s="27"/>
       <c r="M41" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="N41" s="25" t="s">
         <v>353</v>
-      </c>
-      <c r="N41" s="25" t="s">
-        <v>354</v>
       </c>
       <c r="O41" s="26" t="s">
         <v>210</v>
@@ -5952,7 +5898,7 @@
         <v>212</v>
       </c>
       <c r="N42" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O42" s="20" t="s">
         <v>226</v>
@@ -6063,7 +6009,7 @@
         <v>223</v>
       </c>
       <c r="D43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E43" t="s">
         <v>215</v>
@@ -6078,7 +6024,7 @@
         <v>270</v>
       </c>
       <c r="I43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J43">
         <v>3</v>
@@ -6087,13 +6033,13 @@
         <v>229</v>
       </c>
       <c r="L43" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="M43" t="s">
         <v>238</v>
       </c>
       <c r="N43" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AC43" t="s">
         <v>290</v>
@@ -6183,10 +6129,10 @@
         <v>229</v>
       </c>
       <c r="L44" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O44" s="26" t="s">
         <v>210</v>
@@ -6237,10 +6183,10 @@
         <v>229</v>
       </c>
       <c r="L45" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N45" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O45" s="20" t="s">
         <v>210</v>
@@ -6360,13 +6306,13 @@
       </c>
       <c r="B46" t="str">
         <f>IF(OR($A45=$A46,ISBLANK($A46)),"",IF(ISERR(SEARCH("cell-based",E46)),IF(AND(ISERR(SEARCH("biochem",E46)),ISERR(SEARCH("protein",E46)),ISERR(SEARCH("nucleic",E46))),"",IF(ISERR(SEARCH("target",G46)),"Define a Target component","")),IF(ISERR(SEARCH("cell",G46)),"Define a Cell component",""))&amp;IF(ISERR(SEARCH("small-molecule",E46)),IF(ISBLANK(K46), "Need a Detector Role",""),"")&amp;IF(ISERR(SEARCH("fluorescence",L46)),"",IF(ISBLANK(S46), "Need Emission",IF(ISBLANK(R46), "Need Excitation","")))&amp;IF(ISERR(SEARCH("absorbance",L46)),"",IF(ISBLANK(T46), "Need Absorbance","")))</f>
-        <v/>
+        <v>Need a Detector Role</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>230</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>215</v>
@@ -6381,22 +6327,18 @@
         <v>270</v>
       </c>
       <c r="I46" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="J46" s="8">
-        <v>2000</v>
-      </c>
-      <c r="K46" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O46" s="8"/>
       <c r="P46" s="8"/>
@@ -6413,7 +6355,7 @@
       <c r="AA46" s="8"/>
       <c r="AB46" s="8"/>
       <c r="AC46" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AD46" s="5" t="s">
         <v>297</v>
@@ -6508,7 +6450,7 @@
         <v>212</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O47" s="8" t="s">
         <v>226</v>
@@ -6557,7 +6499,7 @@
         <v>273</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J48" s="8">
         <v>1</v>
@@ -6566,7 +6508,7 @@
         <v>225</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AC48" s="11"/>
       <c r="AD48" s="12"/>
@@ -6582,7 +6524,7 @@
         <v>273</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J49" s="20">
         <v>100</v>
@@ -6591,7 +6533,7 @@
         <v>225</v>
       </c>
       <c r="N49" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AC49" s="24"/>
       <c r="AD49" s="18"/>
@@ -6612,7 +6554,7 @@
         <v>219</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>262</v>
@@ -6628,13 +6570,13 @@
         <v>249</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N50" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O50" s="8"/>
       <c r="P50" s="8"/>
@@ -6737,10 +6679,10 @@
         <v>249</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N51" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O51" s="8" t="s">
         <v>210</v>
@@ -6749,7 +6691,7 @@
         <v>213</v>
       </c>
       <c r="Q51" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R51" s="8" t="s">
         <v>206</v>
@@ -6786,14 +6728,10 @@
       <c r="H52" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="J52" s="26">
-        <v>1000</v>
-      </c>
-      <c r="K52" s="27" t="s">
-        <v>314</v>
-      </c>
+      <c r="J52" s="26"/>
+      <c r="K52" s="27"/>
       <c r="N52" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O52" s="8" t="s">
         <v>210</v>
@@ -6802,7 +6740,7 @@
         <v>213</v>
       </c>
       <c r="Q52" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R52" s="8" t="s">
         <v>206</v>
@@ -6840,16 +6778,16 @@
         <v>255</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J53" s="26">
         <v>50</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O53" s="8" t="s">
         <v>210</v>
@@ -6858,7 +6796,7 @@
         <v>213</v>
       </c>
       <c r="Q53" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R53" s="8" t="s">
         <v>206</v>
@@ -6902,17 +6840,17 @@
         <v>273</v>
       </c>
       <c r="I54" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J54" s="20">
         <v>10</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M54" s="17"/>
       <c r="N54" s="20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AC54" s="24"/>
       <c r="AD54" s="18"/>
@@ -6951,13 +6889,13 @@
         <v>1</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>312</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N55" s="8" t="s">
         <v>312</v>
@@ -7068,7 +7006,7 @@
         <v>273</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J56" s="8">
         <v>50</v>
@@ -7132,7 +7070,7 @@
         <v>273</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J57" s="20">
         <v>9</v>
@@ -7141,7 +7079,7 @@
         <v>225</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AC57" s="18"/>
       <c r="AD57" s="18"/>
@@ -7314,7 +7252,7 @@
         <v>230</v>
       </c>
       <c r="D60" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E60" t="s">
         <v>215</v>
@@ -7329,7 +7267,7 @@
         <v>270</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J60">
         <v>30</v>
@@ -7338,13 +7276,13 @@
         <v>246</v>
       </c>
       <c r="L60" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M60" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N60" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AC60" s="4" t="s">
         <v>291</v>
@@ -7442,7 +7380,7 @@
         <v>225</v>
       </c>
       <c r="N61" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O61" s="23" t="s">
         <v>226</v>
@@ -7497,7 +7435,7 @@
         <v>230</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>215</v>
@@ -7512,7 +7450,7 @@
         <v>270</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J62" s="8">
         <v>0.25</v>
@@ -7521,13 +7459,13 @@
         <v>246</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M62" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N62" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O62" s="8"/>
       <c r="P62" s="8"/>
@@ -7639,7 +7577,7 @@
         <v>212</v>
       </c>
       <c r="N63" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O63" s="8" t="s">
         <v>226</v>
@@ -7658,16 +7596,11 @@
         <v>273</v>
       </c>
       <c r="I64" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="J64" s="20">
-        <v>8</v>
-      </c>
-      <c r="K64" s="21" t="s">
-        <v>314</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="K64" s="21"/>
       <c r="N64" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O64" s="20" t="s">
         <v>210</v>
@@ -7816,7 +7749,7 @@
         <v>219</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>262</v>
@@ -7832,13 +7765,13 @@
         <v>249</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M66" s="8" t="s">
         <v>242</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O66" s="8"/>
       <c r="P66" s="8"/>
@@ -7953,11 +7886,11 @@
         <v>249</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M67" s="8"/>
       <c r="N67" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O67" s="8" t="s">
         <v>210</v>
@@ -7966,7 +7899,7 @@
         <v>213</v>
       </c>
       <c r="Q67" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R67" s="8" t="s">
         <v>206</v>
@@ -8045,16 +7978,12 @@
         <v>255</v>
       </c>
       <c r="I68" s="8"/>
-      <c r="J68" s="26">
-        <v>1000</v>
-      </c>
-      <c r="K68" s="27" t="s">
-        <v>314</v>
-      </c>
+      <c r="J68" s="26"/>
+      <c r="K68" s="27"/>
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
       <c r="N68" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O68" s="8" t="s">
         <v>210</v>
@@ -8063,7 +7992,7 @@
         <v>213</v>
       </c>
       <c r="Q68" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R68" s="8" t="s">
         <v>206</v>
@@ -8142,18 +8071,18 @@
         <v>255</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J69" s="26">
         <v>50</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
       <c r="N69" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O69" s="8" t="s">
         <v>210</v>
@@ -8162,7 +8091,7 @@
         <v>213</v>
       </c>
       <c r="Q69" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R69" s="8" t="s">
         <v>206</v>
@@ -8253,17 +8182,17 @@
         <v>273</v>
       </c>
       <c r="I70" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J70" s="20">
         <v>10</v>
       </c>
       <c r="K70" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M70" s="17"/>
       <c r="N70" s="20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AC70" s="24"/>
       <c r="AD70" s="18"/>
@@ -8286,7 +8215,7 @@
         <v>230</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>215</v>
@@ -8301,7 +8230,7 @@
         <v>270</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J71" s="8">
         <v>0.25</v>
@@ -8310,13 +8239,13 @@
         <v>246</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M71" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N71" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O71" s="8"/>
       <c r="P71" s="8"/>
@@ -8439,7 +8368,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
       <c r="N72" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O72" s="8" t="s">
         <v>226</v>
@@ -8507,18 +8436,14 @@
         <v>273</v>
       </c>
       <c r="I73" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="J73" s="20">
-        <v>8</v>
-      </c>
-      <c r="K73" s="21" t="s">
-        <v>314</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="J73" s="20"/>
+      <c r="K73" s="21"/>
       <c r="L73" s="20"/>
       <c r="M73" s="20"/>
       <c r="N73" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O73" s="20" t="s">
         <v>210</v>
@@ -8601,7 +8526,7 @@
         <v>230</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>215</v>
@@ -8616,7 +8541,7 @@
         <v>270</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J74" s="8">
         <v>13</v>
@@ -8625,13 +8550,13 @@
         <v>229</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M74" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N74" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O74" s="8"/>
       <c r="P74" s="8"/>
@@ -8735,7 +8660,7 @@
         <v>273</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J75" s="8">
         <v>500</v>
@@ -8746,7 +8671,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
       <c r="N75" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O75" s="8" t="s">
         <v>226</v>
@@ -8810,16 +8735,11 @@
         <v>273</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="J76" s="20">
-        <v>3</v>
-      </c>
-      <c r="K76" s="21" t="s">
-        <v>314</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="K76" s="21"/>
       <c r="N76" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O76" s="20" t="s">
         <v>210</v>
@@ -8893,7 +8813,7 @@
         <v>230</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>215</v>
@@ -8908,7 +8828,7 @@
         <v>270</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J77" s="8">
         <v>13</v>
@@ -8917,13 +8837,13 @@
         <v>229</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M77" s="8" t="s">
         <v>238</v>
       </c>
       <c r="N77" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O77" s="8"/>
       <c r="P77" s="8"/>
@@ -9033,7 +8953,7 @@
         <v>273</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J78" s="8">
         <v>500</v>
@@ -9042,7 +8962,7 @@
         <v>212</v>
       </c>
       <c r="N78" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O78" s="8" t="s">
         <v>226</v>
@@ -9086,18 +9006,14 @@
         <v>273</v>
       </c>
       <c r="I79" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="J79" s="20">
-        <v>3</v>
-      </c>
-      <c r="K79" s="21" t="s">
-        <v>314</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="J79" s="20"/>
+      <c r="K79" s="21"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>
       <c r="N79" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O79" s="20" t="s">
         <v>210</v>
@@ -9146,7 +9062,7 @@
         <v>1</v>
       </c>
       <c r="AI79" s="37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AJ79" s="20"/>
       <c r="AK79" s="20"/>
@@ -9202,13 +9118,13 @@
         <v>249</v>
       </c>
       <c r="L80" s="34" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M80" s="34" t="s">
         <v>242</v>
       </c>
       <c r="N80" s="34" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S80" s="34" t="s">
         <v>228</v>
@@ -9288,17 +9204,12 @@
       <c r="H81" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="J81" s="26">
-        <v>2</v>
-      </c>
-      <c r="K81" s="27" t="s">
-        <v>314</v>
-      </c>
+      <c r="K81" s="27"/>
       <c r="L81" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N81" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O81" s="26" t="s">
         <v>210</v>
@@ -9353,19 +9264,14 @@
         <v>255</v>
       </c>
       <c r="I82" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="J82" s="20">
-        <v>200000</v>
-      </c>
-      <c r="K82" s="21" t="s">
-        <v>314</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="K82" s="21"/>
       <c r="L82" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N82" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AC82" s="24"/>
       <c r="AD82" s="24"/>
@@ -9403,13 +9309,13 @@
         <v>1</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>312</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N83" s="8" t="s">
         <v>312</v>
@@ -9520,7 +9426,7 @@
         <v>273</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J84" s="8">
         <v>50</v>
@@ -9604,7 +9510,7 @@
         <v>273</v>
       </c>
       <c r="I85" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J85" s="20">
         <v>9</v>
@@ -9615,7 +9521,7 @@
       <c r="L85" s="20"/>
       <c r="M85" s="20"/>
       <c r="N85" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O85" s="20"/>
       <c r="P85" s="20"/>

</xml_diff>